<commit_message>
Updated in the latest version of SimpleBox4Nano.
</commit_message>
<xml_diff>
--- a/SimpleBox4Nano/src/main/webapp/resources/templates/nanomaterials.xlsx
+++ b/SimpleBox4Nano/src/main/webapp/resources/templates/nanomaterials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\git\nanosolveit\NanoSolveIT\src\main\webapp\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\git\SimpleBox4Nano\SimpleBox4Nano\src\main\webapp\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7887BCBB-5A72-4994-B11D-F357363DD588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5818AC-0C0F-4B36-B024-1A21CC3A0B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -30,14 +30,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -537,7 +529,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -562,8 +554,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -591,11 +589,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -630,9 +637,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -648,9 +652,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -659,15 +660,9 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -683,6 +678,7 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,7 +701,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="version"/>
@@ -23209,7 +23205,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="version"/>
@@ -23518,8 +23514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ES11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
-      <selection activeCell="BC20" sqref="BC20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23570,385 +23566,385 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:127" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="T1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="U1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="V1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="W1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="X1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Y1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="Z1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AA1" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AB1" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="AC1" s="13" t="s">
+      <c r="AC1" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AD1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="15" t="s">
+      <c r="AE1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="16" t="s">
+      <c r="AF1" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="13" t="s">
+      <c r="AG1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="13" t="s">
+      <c r="AH1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="13" t="s">
+      <c r="AI1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" s="13" t="s">
+      <c r="AJ1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" s="13" t="s">
+      <c r="AK1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" s="13" t="s">
+      <c r="AL1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" s="13" t="s">
+      <c r="AM1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="AN1" s="13" t="s">
+      <c r="AN1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="AO1" s="13" t="s">
+      <c r="AO1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" s="13" t="s">
+      <c r="AP1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="AQ1" s="13" t="s">
+      <c r="AQ1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AR1" s="13" t="s">
+      <c r="AR1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="AS1" s="13" t="s">
+      <c r="AS1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="AT1" s="13" t="s">
+      <c r="AT1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="AU1" s="13" t="s">
+      <c r="AU1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="AV1" s="13" t="s">
+      <c r="AV1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="AW1" s="13" t="s">
+      <c r="AW1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="AX1" s="13" t="s">
+      <c r="AX1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AY1" s="13" t="s">
+      <c r="AY1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="AZ1" s="13" t="s">
+      <c r="AZ1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="BA1" s="13" t="s">
+      <c r="BA1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="BB1" s="13" t="s">
+      <c r="BB1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="BC1" s="13" t="s">
+      <c r="BC1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="BD1" s="13" t="s">
+      <c r="BD1" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="BE1" s="13" t="s">
+      <c r="BE1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="BF1" s="13" t="s">
+      <c r="BF1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="BG1" s="13" t="s">
+      <c r="BG1" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="BH1" s="13" t="s">
+      <c r="BH1" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="BI1" s="13" t="s">
+      <c r="BI1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="BJ1" s="13" t="s">
+      <c r="BJ1" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="BK1" s="13" t="s">
+      <c r="BK1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="BL1" s="13" t="s">
+      <c r="BL1" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="BM1" s="13" t="s">
+      <c r="BM1" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="BN1" s="13" t="s">
+      <c r="BN1" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="BO1" s="13" t="s">
+      <c r="BO1" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="BP1" s="13" t="s">
+      <c r="BP1" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="BQ1" s="13" t="s">
+      <c r="BQ1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="BR1" s="13" t="s">
+      <c r="BR1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="BS1" s="13" t="s">
+      <c r="BS1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="BT1" s="13" t="s">
+      <c r="BT1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="BU1" s="13" t="s">
+      <c r="BU1" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="BV1" s="13" t="s">
+      <c r="BV1" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="BW1" s="13" t="s">
+      <c r="BW1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="BX1" s="13" t="s">
+      <c r="BX1" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="BY1" s="13" t="s">
+      <c r="BY1" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="BZ1" s="13" t="s">
+      <c r="BZ1" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="CA1" s="13" t="s">
+      <c r="CA1" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="CB1" s="13" t="s">
+      <c r="CB1" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="CC1" s="13" t="s">
+      <c r="CC1" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="CD1" s="13" t="s">
+      <c r="CD1" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="CE1" s="27" t="s">
+      <c r="CE1" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="CF1" s="27" t="s">
+      <c r="CF1" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="CG1" s="27" t="s">
+      <c r="CG1" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="CH1" s="27" t="s">
+      <c r="CH1" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="CI1" s="27" t="s">
+      <c r="CI1" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="CJ1" s="27" t="s">
+      <c r="CJ1" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="CK1" s="27" t="s">
+      <c r="CK1" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="CL1" s="27" t="s">
+      <c r="CL1" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="CM1" s="27" t="s">
+      <c r="CM1" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="CN1" s="27" t="s">
+      <c r="CN1" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="CO1" s="27" t="s">
+      <c r="CO1" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="CP1" s="27" t="s">
+      <c r="CP1" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="CQ1" s="27" t="s">
+      <c r="CQ1" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="CR1" s="27" t="s">
+      <c r="CR1" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="CS1" s="27" t="s">
+      <c r="CS1" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="CT1" s="27" t="s">
+      <c r="CT1" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="CU1" s="27" t="s">
+      <c r="CU1" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="CV1" s="27" t="s">
+      <c r="CV1" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="CW1" s="27" t="s">
+      <c r="CW1" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="CX1" s="27" t="s">
+      <c r="CX1" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="CY1" s="27" t="s">
+      <c r="CY1" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="CZ1" s="27" t="s">
+      <c r="CZ1" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="DA1" s="27" t="s">
+      <c r="DA1" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="DB1" s="28" t="s">
+      <c r="DB1" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="DC1" s="28" t="s">
+      <c r="DC1" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="DD1" s="28" t="s">
+      <c r="DD1" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="DE1" s="28" t="s">
+      <c r="DE1" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="DF1" s="28" t="s">
+      <c r="DF1" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="DG1" s="28" t="s">
+      <c r="DG1" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="DH1" s="28" t="s">
+      <c r="DH1" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="DI1" s="28" t="s">
+      <c r="DI1" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="DJ1" s="28" t="s">
+      <c r="DJ1" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="DK1" s="28" t="s">
+      <c r="DK1" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="DL1" s="28" t="s">
+      <c r="DL1" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="DM1" s="28" t="s">
+      <c r="DM1" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="DN1" s="28" t="s">
+      <c r="DN1" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="DO1" s="28" t="s">
+      <c r="DO1" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="DP1" s="28" t="s">
+      <c r="DP1" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="DQ1" s="28" t="s">
+      <c r="DQ1" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="DR1" s="28" t="s">
+      <c r="DR1" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="DS1" s="28" t="s">
+      <c r="DS1" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="DT1" s="28" t="s">
+      <c r="DT1" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="DU1" s="28" t="s">
+      <c r="DU1" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="DV1" s="28" t="s">
+      <c r="DV1" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="DW1" s="28" t="s">
+      <c r="DW1" s="24" t="s">
         <v>151</v>
       </c>
     </row>
@@ -24040,7 +24036,7 @@
       <c r="AC2" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="AD2" s="20" t="s">
+      <c r="AD2" s="18" t="s">
         <v>80</v>
       </c>
       <c r="AE2" s="10" t="s">
@@ -24199,139 +24195,139 @@
       <c r="CD2" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="CE2" s="22" t="s">
+      <c r="CE2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CF2" s="22" t="s">
+      <c r="CF2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CG2" s="22" t="s">
+      <c r="CG2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CH2" s="22" t="s">
+      <c r="CH2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CI2" s="22" t="s">
+      <c r="CI2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CJ2" s="22" t="s">
+      <c r="CJ2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CK2" s="22" t="s">
+      <c r="CK2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CL2" s="22" t="s">
+      <c r="CL2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CM2" s="22" t="s">
+      <c r="CM2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CN2" s="22" t="s">
+      <c r="CN2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CO2" s="22" t="s">
+      <c r="CO2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CP2" s="22" t="s">
+      <c r="CP2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CQ2" s="22" t="s">
+      <c r="CQ2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CR2" s="22" t="s">
+      <c r="CR2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CS2" s="22" t="s">
+      <c r="CS2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CT2" s="22" t="s">
+      <c r="CT2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CU2" s="22" t="s">
+      <c r="CU2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CV2" s="22" t="s">
+      <c r="CV2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CW2" s="22" t="s">
+      <c r="CW2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CX2" s="22" t="s">
+      <c r="CX2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CY2" s="22" t="s">
+      <c r="CY2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="CZ2" s="22" t="s">
+      <c r="CZ2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DA2" s="22" t="s">
+      <c r="DA2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DB2" s="17" t="s">
+      <c r="DB2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DC2" s="17" t="s">
+      <c r="DC2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DD2" s="22" t="s">
+      <c r="DD2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DE2" s="22" t="s">
+      <c r="DE2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DF2" s="22" t="s">
+      <c r="DF2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DG2" s="22" t="s">
+      <c r="DG2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DH2" s="22" t="s">
+      <c r="DH2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DI2" s="22" t="s">
+      <c r="DI2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DJ2" s="22" t="s">
+      <c r="DJ2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DK2" s="22" t="s">
+      <c r="DK2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DL2" s="22" t="s">
+      <c r="DL2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DM2" s="22" t="s">
+      <c r="DM2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DN2" s="22" t="s">
+      <c r="DN2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DO2" s="22" t="s">
+      <c r="DO2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DP2" s="22" t="s">
+      <c r="DP2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DQ2" s="22" t="s">
+      <c r="DQ2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DR2" s="22" t="s">
+      <c r="DR2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DS2" s="22" t="s">
+      <c r="DS2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DT2" s="22" t="s">
+      <c r="DT2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DU2" s="22" t="s">
+      <c r="DU2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DV2" s="22" t="s">
+      <c r="DV2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="DW2" s="22" t="s">
+      <c r="DW2" s="16" t="s">
         <v>84</v>
       </c>
     </row>
@@ -24423,7 +24419,7 @@
       <c r="AC3" s="9">
         <v>0</v>
       </c>
-      <c r="AD3" s="20">
+      <c r="AD3" s="18">
         <v>0</v>
       </c>
       <c r="AE3" s="10">
@@ -24582,139 +24578,139 @@
       <c r="CD3" s="9">
         <v>0</v>
       </c>
-      <c r="CE3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CF3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CG3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CH3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CI3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CJ3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CK3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CL3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CM3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CN3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CO3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CP3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CQ3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CR3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CS3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CT3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CU3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CV3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CW3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CX3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CY3" s="22">
-        <v>0</v>
-      </c>
-      <c r="CZ3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DA3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DB3" s="17">
-        <v>0</v>
-      </c>
-      <c r="DC3" s="17">
-        <v>0</v>
-      </c>
-      <c r="DD3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DE3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DF3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DG3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DH3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DI3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DJ3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DK3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DL3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DM3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DN3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DO3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DP3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DQ3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DR3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DS3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DT3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DU3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DV3" s="22">
-        <v>0</v>
-      </c>
-      <c r="DW3" s="22">
+      <c r="CE3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CF3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CG3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CH3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CI3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CJ3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CK3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CL3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CM3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CN3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CQ3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CR3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CS3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CT3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CU3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CV3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CW3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CX3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CY3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CZ3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DA3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DB3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DC3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DD3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DE3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DF3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DG3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DH3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DI3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DJ3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DK3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DL3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DM3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DN3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DO3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DP3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DQ3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DR3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DS3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DT3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DU3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DV3" s="16">
+        <v>0</v>
+      </c>
+      <c r="DW3" s="16">
         <v>0</v>
       </c>
     </row>
@@ -24806,7 +24802,7 @@
       <c r="AC4" s="9">
         <v>0</v>
       </c>
-      <c r="AD4" s="20">
+      <c r="AD4" s="18">
         <v>75</v>
       </c>
       <c r="AE4" s="10">
@@ -24965,139 +24961,139 @@
       <c r="CD4" s="9">
         <v>0</v>
       </c>
-      <c r="CE4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CF4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CG4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CH4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CI4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CJ4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CK4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CL4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CM4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CN4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CO4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CP4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CQ4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CR4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CS4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CT4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CU4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CV4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CW4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CX4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CY4" s="22">
-        <v>0</v>
-      </c>
-      <c r="CZ4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DA4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DB4" s="17">
-        <v>0</v>
-      </c>
-      <c r="DC4" s="17">
-        <v>0</v>
-      </c>
-      <c r="DD4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DE4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DF4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DG4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DH4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DI4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DJ4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DK4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DL4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DM4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DN4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DO4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DP4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DQ4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DR4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DS4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DT4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DU4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DV4" s="22">
-        <v>0</v>
-      </c>
-      <c r="DW4" s="22">
+      <c r="CE4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CF4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CG4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CH4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CI4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CJ4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CK4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CL4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CM4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CN4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CQ4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CR4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CS4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CT4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CU4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CV4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CW4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CX4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CY4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CZ4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DA4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DB4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DC4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DD4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DE4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DF4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DG4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DH4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DI4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DJ4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DK4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DL4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DM4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DN4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DO4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DP4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DQ4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DR4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DS4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DT4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DU4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DV4" s="16">
+        <v>0</v>
+      </c>
+      <c r="DW4" s="16">
         <v>0</v>
       </c>
     </row>
@@ -25189,7 +25185,7 @@
       <c r="AC5" s="9">
         <v>0</v>
       </c>
-      <c r="AD5" s="20">
+      <c r="AD5" s="18">
         <v>9.5</v>
       </c>
       <c r="AE5" s="9">
@@ -25348,139 +25344,139 @@
       <c r="CD5" s="9">
         <v>0</v>
       </c>
-      <c r="CE5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CF5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CG5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CH5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CI5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CJ5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CK5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CL5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CM5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CN5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CO5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CP5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CQ5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CR5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CS5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CT5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CU5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CV5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CW5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CX5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CY5" s="22">
-        <v>0</v>
-      </c>
-      <c r="CZ5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DA5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DB5" s="17">
-        <v>0</v>
-      </c>
-      <c r="DC5" s="17">
-        <v>0</v>
-      </c>
-      <c r="DD5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DE5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DF5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DG5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DH5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DI5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DJ5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DK5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DL5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DM5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DN5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DO5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DP5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DQ5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DR5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DS5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DT5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DU5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DV5" s="22">
-        <v>0</v>
-      </c>
-      <c r="DW5" s="22">
+      <c r="CE5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CF5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CG5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CH5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CI5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CJ5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CK5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CL5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CM5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CN5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CQ5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CR5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CS5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CT5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CU5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CV5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CW5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CX5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CY5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CZ5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DA5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DB5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DC5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DD5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DE5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DF5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DG5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DH5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DI5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DJ5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DK5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DL5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DM5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DN5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DO5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DP5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DQ5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DR5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DS5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DT5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DU5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DV5" s="16">
+        <v>0</v>
+      </c>
+      <c r="DW5" s="16">
         <v>0</v>
       </c>
     </row>
@@ -25572,7 +25568,7 @@
       <c r="AC6" s="9">
         <v>0</v>
       </c>
-      <c r="AD6" s="20">
+      <c r="AD6" s="18">
         <v>75</v>
       </c>
       <c r="AE6" s="9">
@@ -25731,139 +25727,139 @@
       <c r="CD6" s="9">
         <v>1.1800000000000001E-5</v>
       </c>
-      <c r="CE6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CF6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CG6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CH6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CI6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CJ6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CK6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CL6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CM6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CN6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CO6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CP6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CQ6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CR6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CS6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CT6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CU6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CV6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CW6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CX6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CY6" s="22">
-        <v>0</v>
-      </c>
-      <c r="CZ6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DA6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DB6" s="17">
-        <v>0</v>
-      </c>
-      <c r="DC6" s="17">
-        <v>0</v>
-      </c>
-      <c r="DD6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DE6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DF6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DG6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DH6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DI6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DJ6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DK6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DL6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DM6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DN6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DO6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DP6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DQ6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DR6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DS6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DT6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DU6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DV6" s="22">
-        <v>0</v>
-      </c>
-      <c r="DW6" s="22">
+      <c r="CE6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CF6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CG6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CH6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CI6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CJ6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CK6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CL6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CM6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CN6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CQ6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CR6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CS6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CT6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CU6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CV6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CW6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CX6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CY6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CZ6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DA6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DB6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DC6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DD6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DE6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DF6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DG6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DH6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DI6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DJ6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DK6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DL6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DM6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DN6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DO6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DP6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DQ6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DR6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DS6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DT6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DU6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DV6" s="16">
+        <v>0</v>
+      </c>
+      <c r="DW6" s="16">
         <v>0</v>
       </c>
     </row>
@@ -25955,7 +25951,7 @@
       <c r="AC7" s="9">
         <v>0</v>
       </c>
-      <c r="AD7" s="20">
+      <c r="AD7" s="18">
         <v>75</v>
       </c>
       <c r="AE7" s="9">
@@ -26051,58 +26047,58 @@
       <c r="BI7" s="9">
         <v>1.6500000000000001E-6</v>
       </c>
-      <c r="BJ7" s="29">
+      <c r="BJ7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="BK7" s="29">
+      <c r="BK7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="BL7" s="29">
+      <c r="BL7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="BM7" s="29">
+      <c r="BM7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="BN7" s="29">
+      <c r="BN7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="BO7" s="29">
+      <c r="BO7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="BP7" s="29">
+      <c r="BP7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="BQ7" s="29">
+      <c r="BQ7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="BR7" s="29">
+      <c r="BR7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="BS7" s="29">
+      <c r="BS7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="BT7" s="29">
+      <c r="BT7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="BU7" s="29">
+      <c r="BU7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="BV7" s="29">
+      <c r="BV7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="BW7" s="29">
+      <c r="BW7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="BX7" s="29">
+      <c r="BX7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="BY7" s="29">
+      <c r="BY7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="BZ7" s="29">
+      <c r="BZ7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="CA7" s="29">
+      <c r="CA7" s="25">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="CB7" s="9">
@@ -26114,139 +26110,139 @@
       <c r="CD7" s="9">
         <v>1.6500000000000001E-6</v>
       </c>
-      <c r="CE7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CF7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CG7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CH7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CI7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CJ7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CK7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CL7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CM7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CN7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CO7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CP7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CQ7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CR7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CS7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CT7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CU7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CV7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CW7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CX7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CY7" s="22">
-        <v>0</v>
-      </c>
-      <c r="CZ7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DA7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DB7" s="17">
-        <v>0</v>
-      </c>
-      <c r="DC7" s="17">
-        <v>0</v>
-      </c>
-      <c r="DD7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DE7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DF7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DG7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DH7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DI7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DJ7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DK7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DL7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DM7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DN7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DO7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DP7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DQ7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DR7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DS7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DT7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DU7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DV7" s="22">
-        <v>0</v>
-      </c>
-      <c r="DW7" s="22">
+      <c r="CE7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CF7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CG7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CH7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CI7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CJ7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CK7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CL7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CM7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CN7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CQ7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CR7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CS7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CT7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CU7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CV7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CW7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CX7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CY7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CZ7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DA7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DB7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DC7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DD7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DE7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DF7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DG7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DH7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DI7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DJ7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DK7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DL7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DM7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DN7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DO7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DP7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DQ7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DR7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DS7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DT7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DU7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DV7" s="16">
+        <v>0</v>
+      </c>
+      <c r="DW7" s="16">
         <v>0</v>
       </c>
     </row>
@@ -26338,7 +26334,7 @@
       <c r="AC8" s="9">
         <v>0</v>
       </c>
-      <c r="AD8" s="20">
+      <c r="AD8" s="18">
         <v>5</v>
       </c>
       <c r="AE8" s="9">
@@ -26497,139 +26493,139 @@
       <c r="CD8" s="9">
         <v>0</v>
       </c>
-      <c r="CE8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CF8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CG8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CH8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CI8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CJ8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CK8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CL8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CM8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CN8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CO8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CP8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CQ8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CR8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CS8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CT8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CU8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CV8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CW8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CX8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CY8" s="22">
-        <v>0</v>
-      </c>
-      <c r="CZ8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DA8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DB8" s="17">
-        <v>0</v>
-      </c>
-      <c r="DC8" s="17">
-        <v>0</v>
-      </c>
-      <c r="DD8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DE8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DF8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DG8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DH8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DI8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DJ8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DK8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DL8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DM8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DN8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DO8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DP8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DQ8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DR8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DS8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DT8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DU8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DV8" s="22">
-        <v>0</v>
-      </c>
-      <c r="DW8" s="22">
+      <c r="CE8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CF8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CG8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CH8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CI8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CJ8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CK8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CL8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CM8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CN8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CQ8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CR8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CS8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CT8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CU8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CV8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CW8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CX8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CY8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CZ8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DA8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DB8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DC8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DD8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DE8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DF8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DG8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DH8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DI8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DJ8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DK8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DL8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DM8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DN8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DO8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DP8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DQ8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DR8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DS8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DT8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DU8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DV8" s="16">
+        <v>0</v>
+      </c>
+      <c r="DW8" s="16">
         <v>0</v>
       </c>
     </row>
@@ -26721,7 +26717,7 @@
       <c r="AC9" s="9">
         <v>0</v>
       </c>
-      <c r="AD9" s="20">
+      <c r="AD9" s="18">
         <v>5</v>
       </c>
       <c r="AE9" s="9">
@@ -26880,522 +26876,522 @@
       <c r="CD9" s="9">
         <v>1.1800000000000001E-5</v>
       </c>
-      <c r="CE9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CF9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CG9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CH9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CI9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CJ9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CK9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CL9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CM9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CN9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CO9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CP9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CQ9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CR9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CS9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CT9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CU9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CV9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CW9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CX9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CY9" s="22">
-        <v>0</v>
-      </c>
-      <c r="CZ9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DA9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DB9" s="17">
-        <v>0</v>
-      </c>
-      <c r="DC9" s="17">
-        <v>0</v>
-      </c>
-      <c r="DD9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DE9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DF9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DG9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DH9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DI9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DJ9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DK9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DL9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DM9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DN9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DO9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DP9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DQ9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DR9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DS9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DT9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DU9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DV9" s="22">
-        <v>0</v>
-      </c>
-      <c r="DW9" s="22">
+      <c r="CE9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CF9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CG9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CH9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CI9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CJ9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CK9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CL9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CM9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CN9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CQ9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CR9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CS9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CT9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CU9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CV9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CW9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CX9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CY9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CZ9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DA9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DB9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DC9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DD9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DE9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DF9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DG9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DH9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DI9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DJ9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DK9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DL9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DM9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DN9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DO9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DP9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DQ9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DR9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DS9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DT9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DU9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DV9" s="16">
+        <v>0</v>
+      </c>
+      <c r="DW9" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:127" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12">
+      <c r="A10" s="9">
         <v>10</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="9">
         <v>0</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="E10" s="12">
-        <v>0</v>
-      </c>
-      <c r="F10" s="12">
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9">
         <v>47.366999999999997</v>
       </c>
-      <c r="G10" s="12">
-        <v>0</v>
-      </c>
-      <c r="H10" s="12">
+      <c r="G10" s="9">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9">
         <v>2.4084152589004067E-36</v>
       </c>
-      <c r="I10" s="12">
-        <v>0</v>
-      </c>
-      <c r="J10" s="12">
+      <c r="I10" s="9">
+        <v>0</v>
+      </c>
+      <c r="J10" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="K10" s="12">
-        <v>0</v>
-      </c>
-      <c r="L10" s="12">
-        <v>0</v>
-      </c>
-      <c r="M10" s="12">
-        <v>0</v>
-      </c>
-      <c r="N10" s="12">
-        <v>0</v>
-      </c>
-      <c r="O10" s="12">
-        <v>0</v>
-      </c>
-      <c r="P10" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="12">
+      <c r="K10" s="9">
+        <v>0</v>
+      </c>
+      <c r="L10" s="9">
+        <v>0</v>
+      </c>
+      <c r="M10" s="9">
+        <v>0</v>
+      </c>
+      <c r="N10" s="9">
+        <v>0</v>
+      </c>
+      <c r="O10" s="9">
+        <v>0</v>
+      </c>
+      <c r="P10" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="R10" s="12">
+      <c r="R10" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="S10" s="12">
+      <c r="S10" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="T10" s="12">
+      <c r="T10" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="U10" s="12">
-        <v>0</v>
-      </c>
-      <c r="V10" s="12">
-        <v>0</v>
-      </c>
-      <c r="W10" s="12">
+      <c r="U10" s="9">
+        <v>0</v>
+      </c>
+      <c r="V10" s="9">
+        <v>0</v>
+      </c>
+      <c r="W10" s="9">
         <v>30000</v>
       </c>
-      <c r="X10" s="12">
+      <c r="X10" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="Y10" s="12">
+      <c r="Y10" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="Z10" s="12">
+      <c r="Z10" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AA10" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="12">
+      <c r="AA10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="9">
         <v>10</v>
       </c>
-      <c r="AC10" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="21">
+      <c r="AC10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="19">
         <v>5</v>
       </c>
-      <c r="AE10" s="12">
+      <c r="AE10" s="9">
         <v>4230</v>
       </c>
-      <c r="AF10" s="12">
+      <c r="AF10" s="9">
         <v>6.9000000000000004E-21</v>
       </c>
-      <c r="AG10" s="12">
+      <c r="AG10" s="9">
         <v>0.02</v>
       </c>
-      <c r="AH10" s="12">
+      <c r="AH10" s="9">
         <v>0.02</v>
       </c>
-      <c r="AI10" s="12">
+      <c r="AI10" s="9">
         <v>0.02</v>
       </c>
-      <c r="AJ10" s="12">
+      <c r="AJ10" s="9">
         <v>0.02</v>
       </c>
-      <c r="AK10" s="12">
+      <c r="AK10" s="9">
         <v>1</v>
       </c>
-      <c r="AL10" s="12">
+      <c r="AL10" s="9">
         <v>1</v>
       </c>
-      <c r="AM10" s="12">
+      <c r="AM10" s="9">
         <v>1</v>
       </c>
-      <c r="AN10" s="12">
+      <c r="AN10" s="9">
         <v>1</v>
       </c>
-      <c r="AO10" s="12">
+      <c r="AO10" s="9">
         <v>0.33600000000000002</v>
       </c>
-      <c r="AP10" s="12">
+      <c r="AP10" s="9">
         <v>0.33600000000000002</v>
       </c>
-      <c r="AQ10" s="12">
+      <c r="AQ10" s="9">
         <v>0.33600000000000002</v>
       </c>
-      <c r="AR10" s="12">
+      <c r="AR10" s="9">
         <v>0.33600000000000002</v>
       </c>
-      <c r="AS10" s="12">
+      <c r="AS10" s="9">
         <v>0.33600000000000002</v>
       </c>
-      <c r="AT10" s="12">
+      <c r="AT10" s="9">
         <v>0.33600000000000002</v>
       </c>
-      <c r="AU10" s="12">
+      <c r="AU10" s="9">
         <v>0.02</v>
       </c>
-      <c r="AV10" s="12">
+      <c r="AV10" s="9">
         <v>0.02</v>
       </c>
-      <c r="AW10" s="12">
+      <c r="AW10" s="9">
         <v>0.02</v>
       </c>
-      <c r="AX10" s="12">
+      <c r="AX10" s="9">
         <v>0.02</v>
       </c>
-      <c r="AY10" s="12">
+      <c r="AY10" s="9">
         <v>1</v>
       </c>
-      <c r="AZ10" s="12">
+      <c r="AZ10" s="9">
         <v>1</v>
       </c>
-      <c r="BA10" s="12">
+      <c r="BA10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BB10" s="12">
+      <c r="BB10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BC10" s="12">
+      <c r="BC10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BD10" s="12">
+      <c r="BD10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BE10" s="12">
+      <c r="BE10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BF10" s="12">
+      <c r="BF10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BG10" s="12">
+      <c r="BG10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BH10" s="12">
+      <c r="BH10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BI10" s="12">
+      <c r="BI10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BJ10" s="12">
+      <c r="BJ10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BK10" s="12">
+      <c r="BK10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BL10" s="12">
+      <c r="BL10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BM10" s="12">
+      <c r="BM10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BN10" s="12">
+      <c r="BN10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BO10" s="12">
+      <c r="BO10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BP10" s="12">
+      <c r="BP10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BQ10" s="12">
+      <c r="BQ10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BR10" s="12">
+      <c r="BR10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BS10" s="12">
+      <c r="BS10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BT10" s="12">
+      <c r="BT10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BU10" s="12">
+      <c r="BU10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BV10" s="12">
+      <c r="BV10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BW10" s="12">
+      <c r="BW10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BX10" s="12">
+      <c r="BX10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BY10" s="12">
+      <c r="BY10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="BZ10" s="12">
+      <c r="BZ10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="CA10" s="12">
+      <c r="CA10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="CB10" s="12">
+      <c r="CB10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="CC10" s="12">
+      <c r="CC10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="CD10" s="12">
+      <c r="CD10" s="9">
         <v>1E-13</v>
       </c>
-      <c r="CE10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CF10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CG10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CH10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CI10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CJ10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CK10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CL10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CM10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CN10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CO10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CP10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CQ10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CR10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CS10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CT10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CU10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CV10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CW10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CX10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CY10" s="23">
-        <v>0</v>
-      </c>
-      <c r="CZ10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DA10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DB10" s="18">
-        <v>0</v>
-      </c>
-      <c r="DC10" s="18">
-        <v>0</v>
-      </c>
-      <c r="DD10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DE10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DF10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DG10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DH10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DI10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DJ10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DK10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DL10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DM10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DN10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DO10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DP10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DQ10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DR10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DS10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DT10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DU10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DV10" s="23">
-        <v>0</v>
-      </c>
-      <c r="DW10" s="23">
+      <c r="CE10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CF10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CG10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CH10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CI10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CJ10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CK10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CL10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CM10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CN10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CQ10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CR10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CS10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CT10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CU10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CV10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CW10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CX10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CY10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CZ10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DA10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DB10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DC10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DD10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DE10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DF10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DG10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DH10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DI10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DJ10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DK10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DL10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DM10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DN10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DO10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DP10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DQ10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DR10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DS10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DT10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DU10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DV10" s="16">
+        <v>0</v>
+      </c>
+      <c r="DW10" s="16">
         <v>0</v>
       </c>
     </row>
@@ -27421,20 +27417,20 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="9">
         <v>2.4084152589004067E-36</v>
       </c>
       <c r="I11" s="1">
         <v>0</v>
       </c>
-      <c r="J11" s="1">
-        <v>0</v>
+      <c r="J11" s="26">
+        <v>9.9999999999999995E-21</v>
       </c>
       <c r="K11" s="1">
         <v>0</v>
       </c>
-      <c r="L11" s="1">
-        <v>0</v>
+      <c r="L11" s="26">
+        <v>2750</v>
       </c>
       <c r="M11" s="1">
         <v>0</v>
@@ -27448,16 +27444,16 @@
       <c r="P11" s="1">
         <v>0</v>
       </c>
-      <c r="Q11" s="12">
+      <c r="Q11" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="R11" s="12">
+      <c r="R11" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="S11" s="12">
+      <c r="S11" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="T11" s="12">
+      <c r="T11" s="9">
         <v>9.9999999999999995E-21</v>
       </c>
       <c r="U11" s="1">
@@ -27466,16 +27462,16 @@
       <c r="V11" s="1">
         <v>0</v>
       </c>
-      <c r="W11" s="12">
+      <c r="W11" s="9">
         <v>30000</v>
       </c>
-      <c r="X11" s="12">
+      <c r="X11" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="Y11" s="12">
+      <c r="Y11" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="Z11" s="12">
+      <c r="Z11" s="9">
         <v>0.33333333333333331</v>
       </c>
       <c r="AA11" s="1">
@@ -27487,75 +27483,75 @@
       <c r="AC11" s="1">
         <v>0</v>
       </c>
-      <c r="AD11" s="24">
+      <c r="AD11" s="20">
         <v>10</v>
       </c>
-      <c r="AE11" s="24">
+      <c r="AE11" s="20">
         <f>4.23*10^3</f>
         <v>4230</v>
       </c>
-      <c r="AF11" s="25">
+      <c r="AF11" s="21">
         <f>6.9*10^-21</f>
         <v>6.9000000000000004E-21</v>
       </c>
-      <c r="AG11" s="25">
+      <c r="AG11" s="21">
         <v>0.1</v>
       </c>
-      <c r="AH11" s="25">
+      <c r="AH11" s="21">
         <v>0.1</v>
       </c>
-      <c r="AI11" s="25">
+      <c r="AI11" s="21">
         <v>0.1</v>
       </c>
-      <c r="AJ11" s="25">
+      <c r="AJ11" s="21">
         <v>0.1</v>
       </c>
-      <c r="AK11" s="12">
+      <c r="AK11" s="9">
         <v>1</v>
       </c>
-      <c r="AL11" s="12">
+      <c r="AL11" s="9">
         <v>1</v>
       </c>
-      <c r="AM11" s="12">
+      <c r="AM11" s="9">
         <v>1</v>
       </c>
-      <c r="AN11" s="12">
+      <c r="AN11" s="9">
         <v>1</v>
       </c>
-      <c r="AO11" s="25">
+      <c r="AO11" s="21">
         <v>0.1</v>
       </c>
-      <c r="AP11" s="25">
+      <c r="AP11" s="21">
         <v>0.1</v>
       </c>
-      <c r="AQ11" s="25">
+      <c r="AQ11" s="21">
         <v>0.1</v>
       </c>
-      <c r="AR11" s="25">
+      <c r="AR11" s="21">
         <v>0.1</v>
       </c>
-      <c r="AS11" s="25">
+      <c r="AS11" s="21">
         <v>0.1</v>
       </c>
-      <c r="AT11" s="25">
+      <c r="AT11" s="21">
         <v>0.1</v>
       </c>
-      <c r="AU11" s="25">
+      <c r="AU11" s="21">
         <v>0.1</v>
       </c>
-      <c r="AV11" s="25">
+      <c r="AV11" s="21">
         <v>0.1</v>
       </c>
-      <c r="AW11" s="25">
+      <c r="AW11" s="21">
         <v>0.1</v>
       </c>
-      <c r="AX11" s="25">
+      <c r="AX11" s="21">
         <v>0.1</v>
       </c>
-      <c r="AY11" s="25">
+      <c r="AY11" s="21">
         <v>1</v>
       </c>
-      <c r="AZ11" s="26">
+      <c r="AZ11" s="22">
         <v>1</v>
       </c>
       <c r="BA11" s="1">
@@ -27785,7 +27781,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="BA11:DW11 E1:AC1048576">
+  <conditionalFormatting sqref="E1:AC10 BA11:DW11 E12:AC1048576 E11:I11 M11:AC11 K11">
     <cfRule type="cellIs" dxfId="0" priority="34" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>